<commit_message>
ejercicio jugando con objetos
</commit_message>
<xml_diff>
--- a/calendario clases.xlsx
+++ b/calendario clases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\curso63RoR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951E3F5B-9901-484D-9AC5-CC959810A250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2FDF59-5A6E-4E0A-AE1F-A5A961DBFB4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FDD01856-7B84-48EF-93CA-ED9D3FC5F03B}"/>
+    <workbookView xWindow="1800" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{FDD01856-7B84-48EF-93CA-ED9D3FC5F03B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>bootstrap</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>funciones jquery, ejercicio ninja</t>
+  </si>
+  <si>
+    <t>ejercicio gato-ninja, uso de for, variable temp, conversacion de compañeros</t>
+  </si>
+  <si>
+    <t>api,JSON anotacion, get es una solicitud</t>
   </si>
 </sst>
 </file>
@@ -449,15 +455,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00196459-BDB9-43F6-8065-8F8295AF10E4}">
-  <dimension ref="B2:E19"/>
+  <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -627,6 +633,22 @@
         <v>17</v>
       </c>
     </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>44364</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>44365</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>